<commit_message>
integrated market data, added date lagging-pushing capability to financial data extract to deal with look-ahead bias
</commit_message>
<xml_diff>
--- a/Economic Data/ONS UK GDP Estimate Monthly.xlsx
+++ b/Economic Data/ONS UK GDP Estimate Monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Renea\OneDrive\Documents\University of Bath\13. Dissertation\Data\Economic Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C1401E-00EB-4A24-8B08-198C1A5C59E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FC91DD-0128-4290-A2B5-FD7EBE947224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,13 +38,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Gross Value Added Index Level - reported 1.5 months after Date</t>
+    <t>2M Lagged Date</t>
   </si>
   <si>
-    <t>Gross Value Added % growth - reported 1.5 months after Date</t>
+    <t>Gross Value Added Level</t>
   </si>
   <si>
-    <t>2M Lagged Date</t>
+    <t>Gross Value Added Growth</t>
   </si>
 </sst>
 </file>
@@ -52,7 +52,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -94,7 +94,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,16 +412,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A287" workbookViewId="0">
-      <selection activeCell="D311" sqref="D311"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -429,13 +429,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>